<commit_message>
Implement parser for complete format language used by TEXT()
</commit_message>
<xml_diff>
--- a/tests/fixtures/text.xlsx
+++ b/tests/fixtures/text.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB09A81C-55D3-4EA6-B042-E3F11D254B14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB38A670-815A-473D-8B69-07EEF8A00166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40125" yWindow="8085" windowWidth="18510" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39630" yWindow="10170" windowWidth="18510" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Text" sheetId="1" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId1"/>
+    <sheet name="TextDates" sheetId="2" r:id="rId2"/>
+    <sheet name="TextNumbers" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
   <si>
     <t>1</t>
   </si>
@@ -101,7 +103,313 @@
     <t>value</t>
   </si>
   <si>
-    <t>FIX ME</t>
+    <t>[m]:s</t>
+  </si>
+  <si>
+    <t>#.###########</t>
+  </si>
+  <si>
+    <t>23.:59</t>
+  </si>
+  <si>
+    <t>23:59.</t>
+  </si>
+  <si>
+    <t>23:59.:0</t>
+  </si>
+  <si>
+    <t>59:9999.012345789</t>
+  </si>
+  <si>
+    <t>60:9999.012345</t>
+  </si>
+  <si>
+    <t>59:9999.012345</t>
+  </si>
+  <si>
+    <t>Final time field with a decimal is seconds</t>
+  </si>
+  <si>
+    <t>23:59.012345</t>
+  </si>
+  <si>
+    <t>#.#####</t>
+  </si>
+  <si>
+    <t>59:10000.0</t>
+  </si>
+  <si>
+    <t>59:9999.0</t>
+  </si>
+  <si>
+    <t>23:60:9999</t>
+  </si>
+  <si>
+    <t>23:59:9999</t>
+  </si>
+  <si>
+    <t>0:0:10000</t>
+  </si>
+  <si>
+    <t>0:0:9999</t>
+  </si>
+  <si>
+    <t>23:10000</t>
+  </si>
+  <si>
+    <t>23:9999</t>
+  </si>
+  <si>
+    <t>24:99</t>
+  </si>
+  <si>
+    <t>23:99</t>
+  </si>
+  <si>
+    <t>non-last limited to 23:59</t>
+  </si>
+  <si>
+    <t>60:99</t>
+  </si>
+  <si>
+    <t>last time field can be &lt; 10,000</t>
+  </si>
+  <si>
+    <t>0:59:99</t>
+  </si>
+  <si>
+    <t>w;x@</t>
+  </si>
+  <si>
+    <t>w;x;z</t>
+  </si>
+  <si>
+    <t>w;x;z@</t>
+  </si>
+  <si>
+    <t>Can mix non keyword text and number</t>
+  </si>
+  <si>
+    <t>#,#"ZZ"#.0z00</t>
+  </si>
+  <si>
+    <t>#,#"ZZ"#.0y00</t>
+  </si>
+  <si>
+    <t>Don’t mix date and number</t>
+  </si>
+  <si>
+    <t>#,#"ZZ"#.0Y00</t>
+  </si>
+  <si>
+    <t>Can mix text and number</t>
+  </si>
+  <si>
+    <t>#,#"ZZ"#.0"YY"00</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>[s].000</t>
+  </si>
+  <si>
+    <t>[s]</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>[m]</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>[h]:m</t>
+  </si>
+  <si>
+    <t>Negative date allowed w/ elapsed</t>
+  </si>
+  <si>
+    <t>[h]</t>
+  </si>
+  <si>
+    <t>can't be &gt; 9999-12-31</t>
+  </si>
+  <si>
+    <t>yy</t>
+  </si>
+  <si>
+    <t>[hh]</t>
+  </si>
+  <si>
+    <t>can be &gt; 9999-12-31 with elapsed</t>
+  </si>
+  <si>
+    <t>"-&gt; "#.00;-#;"SS"m;"ZERO"@</t>
+  </si>
+  <si>
+    <t>;-  ##.0;"ZERO"@;"X"</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>##.00;-  ##.0;"ZERO";-&gt;@&lt;-@</t>
+  </si>
+  <si>
+    <t>##.00;-  ##.0;"ZERO"</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2007-02-03 19:08:07.0123</t>
+  </si>
+  <si>
+    <t>TEXT()</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>#,#"ZZ"#.0"YY"00@</t>
+  </si>
+  <si>
+    <t>Don't mix string replace and number</t>
+  </si>
+  <si>
+    <t>Plugh</t>
+  </si>
+  <si>
+    <t>Empty format gets a '-' w/ negative</t>
+  </si>
+  <si>
+    <t>Empty format pass string through</t>
+  </si>
+  <si>
+    <t>#.#</t>
+  </si>
+  <si>
+    <t>#.##</t>
+  </si>
+  <si>
+    <t>#.###</t>
+  </si>
+  <si>
+    <t>#.###.</t>
+  </si>
+  <si>
+    <t>#.###.#.#.#</t>
+  </si>
+  <si>
+    <t>#,###.##.#</t>
+  </si>
+  <si>
+    <t>#,###.##.##</t>
+  </si>
+  <si>
+    <t>#,###.##.###</t>
+  </si>
+  <si>
+    <t>#,#.##.##,#</t>
+  </si>
+  <si>
+    <t>#,#.##.##\,#</t>
+  </si>
+  <si>
+    <t>0,0.00.0</t>
+  </si>
+  <si>
+    <t>0,#.00.0</t>
+  </si>
+  <si>
+    <t>0,x#.00.0</t>
+  </si>
+  <si>
+    <t>#,0x#.00.0</t>
+  </si>
+  <si>
+    <t>#x,0x#.00.0</t>
+  </si>
+  <si>
+    <t>#x,0,#.00.0</t>
+  </si>
+  <si>
+    <t>,#.00.0</t>
+  </si>
+  <si>
+    <t>.#</t>
+  </si>
+  <si>
+    <t>#.</t>
+  </si>
+  <si>
+    <t>#.###.##.#</t>
+  </si>
+  <si>
+    <t>#.###,x##</t>
+  </si>
+  <si>
+    <t>#.###x,##</t>
+  </si>
+  <si>
+    <t>#.###,x,##</t>
+  </si>
+  <si>
+    <t>#%</t>
+  </si>
+  <si>
+    <t>#.#%</t>
+  </si>
+  <si>
+    <t>#%#</t>
+  </si>
+  <si>
+    <t>%#</t>
+  </si>
+  <si>
+    <t>%#%#%</t>
+  </si>
+  <si>
+    <t>%#%#%#%</t>
+  </si>
+  <si>
+    <t>#.#####00#0</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>1.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$x*y#,##0* </t>
+  </si>
+  <si>
+    <t>##.00;##.0;"ZERO";-&gt;@&lt;-</t>
+  </si>
+  <si>
+    <t>#.########</t>
+  </si>
+  <si>
+    <t>0.########</t>
+  </si>
+  <si>
+    <t>.##</t>
+  </si>
+  <si>
+    <t>.##0</t>
+  </si>
+  <si>
+    <t>#.#######</t>
   </si>
 </sst>
 </file>
@@ -117,18 +425,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,12 +445,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,8 +879,9 @@
         <f>SUBSTITUTE(A2,"y", "q",2)</f>
         <v/>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>17</v>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L21" si="0">TEXT(A2, "#.###")</f>
+        <v>.</v>
       </c>
       <c r="M2" t="str">
         <f>TRIM(A2)</f>
@@ -600,47 +902,47 @@
         <v>#DIV/0!</v>
       </c>
       <c r="B3" t="e">
-        <f t="shared" ref="B3:B21" si="0">_xlfn.CONCAT(A3)</f>
+        <f t="shared" ref="B3:B21" si="1">_xlfn.CONCAT(A3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C3" t="e">
-        <f t="shared" ref="C3:C21" si="1">CONCATENATE(A3)</f>
+        <f t="shared" ref="C3:C21" si="2">CONCATENATE(A3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D3" t="e">
-        <f t="shared" ref="D3:D21" si="2">FIND(A3,A4)</f>
+        <f t="shared" ref="D3:D21" si="3">FIND(A3,A4)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E3" t="e">
-        <f t="shared" ref="E3:E21" si="3">LEFT(A3, 2)</f>
+        <f t="shared" ref="E3:E21" si="4">LEFT(A3, 2)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F3" t="e">
-        <f t="shared" ref="F3:F21" si="4">LEN(A3)</f>
+        <f t="shared" ref="F3:F21" si="5">LEN(A3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G3" t="e">
-        <f t="shared" ref="G3:G21" si="5">LOWER(A3)</f>
+        <f t="shared" ref="G3:G21" si="6">LOWER(A3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H3" t="e">
-        <f t="shared" ref="H3:H21" si="6">MID(A3,1,1)</f>
+        <f t="shared" ref="H3:H21" si="7">MID(A3,1,1)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I3" t="e">
-        <f t="shared" ref="I3:I21" si="7">REPLACE(A3, 1, 3, "z")</f>
+        <f t="shared" ref="I3:I21" si="8">REPLACE(A3, 1, 3, "z")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J3" t="e">
-        <f t="shared" ref="J3:J21" si="8">RIGHT(A3,2)</f>
+        <f t="shared" ref="J3:J21" si="9">RIGHT(A3,2)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K3" t="e">
-        <f t="shared" ref="K3:K20" si="9">SUBSTITUTE(A3,"y", "q",2)</f>
+        <f t="shared" ref="K3:K20" si="10">SUBSTITUTE(A3,"y", "q",2)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L3" t="e">
-        <f t="shared" ref="L2:L21" si="10">TEXT(A3, "#.###")</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M3" t="e">
@@ -661,47 +963,47 @@
         <v>#NUM!</v>
       </c>
       <c r="B4" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C4" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
-      <c r="D4" t="e">
+      <c r="C4" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="E4" t="e">
+      <c r="D4" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="F4" t="e">
+      <c r="E4" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
-      <c r="G4" t="e">
+      <c r="F4" t="e">
         <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
-      <c r="H4" t="e">
+      <c r="G4" t="e">
         <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
-      <c r="I4" t="e">
+      <c r="H4" t="e">
         <f t="shared" si="7"/>
         <v>#NUM!</v>
       </c>
-      <c r="J4" t="e">
+      <c r="I4" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
-      <c r="K4" t="e">
+      <c r="J4" t="e">
         <f t="shared" si="9"/>
         <v>#NUM!</v>
       </c>
+      <c r="K4" t="e">
+        <f t="shared" si="10"/>
+        <v>#NUM!</v>
+      </c>
       <c r="L4" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
       <c r="M4" t="e">
@@ -723,47 +1025,47 @@
         <v>#NAME?</v>
       </c>
       <c r="B5" t="e">
-        <f t="shared" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C5" t="e">
         <f t="shared" si="1"/>
         <v>#NAME?</v>
       </c>
-      <c r="D5" t="e">
+      <c r="C5" t="e">
         <f t="shared" si="2"/>
         <v>#NAME?</v>
       </c>
-      <c r="E5" t="e">
+      <c r="D5" t="e">
         <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
-      <c r="F5" t="e">
+      <c r="E5" t="e">
         <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
-      <c r="G5" t="e">
+      <c r="F5" t="e">
         <f t="shared" si="5"/>
         <v>#NAME?</v>
       </c>
-      <c r="H5" t="e">
+      <c r="G5" t="e">
         <f t="shared" si="6"/>
         <v>#NAME?</v>
       </c>
-      <c r="I5" t="e">
+      <c r="H5" t="e">
         <f t="shared" si="7"/>
         <v>#NAME?</v>
       </c>
-      <c r="J5" t="e">
+      <c r="I5" t="e">
         <f t="shared" si="8"/>
         <v>#NAME?</v>
       </c>
-      <c r="K5" t="e">
+      <c r="J5" t="e">
         <f t="shared" si="9"/>
         <v>#NAME?</v>
       </c>
+      <c r="K5" t="e">
+        <f t="shared" si="10"/>
+        <v>#NAME?</v>
+      </c>
       <c r="L5" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="M5" t="e">
@@ -784,47 +1086,47 @@
         <v>#VALUE!</v>
       </c>
       <c r="B6" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C6" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D6" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E6" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F6" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G6" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H6" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I6" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J6" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K6" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L6" t="e">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C6" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D6" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E6" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F6" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G6" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H6" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I6" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J6" t="e">
-        <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K6" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L6" t="e">
-        <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
       <c r="M6" t="e">
@@ -845,47 +1147,47 @@
         <v>#REF!</v>
       </c>
       <c r="B7" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="C7" t="e">
         <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
-      <c r="D7" t="e">
+      <c r="C7" t="e">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="E7" t="e">
+      <c r="D7" t="e">
         <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
-      <c r="F7" t="e">
+      <c r="E7" t="e">
         <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
-      <c r="G7" t="e">
+      <c r="F7" t="e">
         <f t="shared" si="5"/>
         <v>#REF!</v>
       </c>
-      <c r="H7" t="e">
+      <c r="G7" t="e">
         <f t="shared" si="6"/>
         <v>#REF!</v>
       </c>
-      <c r="I7" t="e">
+      <c r="H7" t="e">
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="J7" t="e">
+      <c r="I7" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="K7" t="e">
+      <c r="J7" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
+      <c r="K7" t="e">
+        <f t="shared" si="10"/>
+        <v>#REF!</v>
+      </c>
       <c r="L7" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
       <c r="M7" t="e">
@@ -906,47 +1208,47 @@
         <v>#NULL!</v>
       </c>
       <c r="B8" t="e">
-        <f t="shared" si="0"/>
-        <v>#NULL!</v>
-      </c>
-      <c r="C8" t="e">
         <f t="shared" si="1"/>
         <v>#NULL!</v>
       </c>
-      <c r="D8" t="e">
+      <c r="C8" t="e">
         <f t="shared" si="2"/>
         <v>#NULL!</v>
       </c>
-      <c r="E8" t="e">
+      <c r="D8" t="e">
         <f t="shared" si="3"/>
         <v>#NULL!</v>
       </c>
-      <c r="F8" t="e">
+      <c r="E8" t="e">
         <f t="shared" si="4"/>
         <v>#NULL!</v>
       </c>
-      <c r="G8" t="e">
+      <c r="F8" t="e">
         <f t="shared" si="5"/>
         <v>#NULL!</v>
       </c>
-      <c r="H8" t="e">
+      <c r="G8" t="e">
         <f t="shared" si="6"/>
         <v>#NULL!</v>
       </c>
-      <c r="I8" t="e">
+      <c r="H8" t="e">
         <f t="shared" si="7"/>
         <v>#NULL!</v>
       </c>
-      <c r="J8" t="e">
+      <c r="I8" t="e">
         <f t="shared" si="8"/>
         <v>#NULL!</v>
       </c>
-      <c r="K8" t="e">
+      <c r="J8" t="e">
         <f t="shared" si="9"/>
         <v>#NULL!</v>
       </c>
+      <c r="K8" t="e">
+        <f t="shared" si="10"/>
+        <v>#NULL!</v>
+      </c>
       <c r="L8" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>#NULL!</v>
       </c>
       <c r="M8" t="e">
@@ -968,47 +1270,47 @@
         <v>#N/A</v>
       </c>
       <c r="B9" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="C9" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D9" t="e">
+      <c r="C9" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="E9" t="e">
+      <c r="D9" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F9" t="e">
+      <c r="E9" t="e">
         <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
-      <c r="G9" t="e">
+      <c r="F9" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H9" t="e">
+      <c r="G9" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I9" t="e">
+      <c r="H9" t="e">
         <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
-      <c r="J9" t="e">
+      <c r="I9" t="e">
         <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
-      <c r="K9" t="e">
+      <c r="J9" t="e">
         <f t="shared" si="9"/>
         <v>#N/A</v>
       </c>
+      <c r="K9" t="e">
+        <f t="shared" si="10"/>
+        <v>#N/A</v>
+      </c>
       <c r="L9" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="M9" t="e">
@@ -1029,47 +1331,48 @@
         <v>-1</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="C10" t="str">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
+      <c r="C10" t="str">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
       <c r="D10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="F10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>z</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="8"/>
-        <v>-1</v>
-      </c>
-      <c r="K10" t="str">
         <f t="shared" si="9"/>
         <v>-1</v>
       </c>
-      <c r="L10" s="4" t="s">
-        <v>17</v>
+      <c r="K10" t="str">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>-1.</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="11"/>
@@ -1089,47 +1392,48 @@
         <v>0</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C11" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="C11" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="D11" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H11" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="H11" t="str">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="I11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>z</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K11" t="str">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="L11" s="4" t="s">
-        <v>17</v>
+      <c r="K11" t="str">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>.</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="11"/>
@@ -1149,47 +1453,48 @@
         <v>1</v>
       </c>
       <c r="B12" t="str">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D12" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="8"/>
+        <v>z</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="L12" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D12" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="7"/>
-        <v>z</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>17</v>
+        <v>1.</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="11"/>
@@ -1209,47 +1514,48 @@
         <v>2</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C13" t="str">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
+      <c r="C13" t="str">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="D13" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="F13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="H13" t="str">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
+      <c r="H13" t="str">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
       <c r="I13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>z</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K13" t="str">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="L13" s="4" t="s">
-        <v>17</v>
+      <c r="K13" t="str">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>2.</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="11"/>
@@ -1269,47 +1575,48 @@
         <v>0</v>
       </c>
       <c r="B14" t="str">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="8"/>
+        <v>z</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="L14" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="7"/>
-        <v>z</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="K14" t="str">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>17</v>
+        <v>1.</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="11"/>
@@ -1329,47 +1636,48 @@
         <v>1</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="C15" t="str">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
+      <c r="C15" t="str">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
       <c r="D15" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="F15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>z</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="8"/>
-        <v>-1</v>
-      </c>
-      <c r="K15" t="str">
         <f t="shared" si="9"/>
         <v>-1</v>
       </c>
-      <c r="L15" s="4" t="s">
-        <v>17</v>
+      <c r="K15" t="str">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>-1.</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="11"/>
@@ -1389,47 +1697,48 @@
         <v>2</v>
       </c>
       <c r="B16" t="str">
+        <f t="shared" si="1"/>
+        <v>XYZZY</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="2"/>
+        <v>XYZZY</v>
+      </c>
+      <c r="D16" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="4"/>
+        <v>XY</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="6"/>
+        <v>xyzzy</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="7"/>
+        <v>X</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="8"/>
+        <v>zZY</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="9"/>
+        <v>ZY</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="10"/>
+        <v>XYZZY</v>
+      </c>
+      <c r="L16" t="str">
         <f t="shared" si="0"/>
         <v>XYZZY</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="1"/>
-        <v>XYZZY</v>
-      </c>
-      <c r="D16" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="3"/>
-        <v>XY</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="G16" t="str">
-        <f t="shared" si="5"/>
-        <v>xyzzy</v>
-      </c>
-      <c r="H16" t="str">
-        <f t="shared" si="6"/>
-        <v>X</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="7"/>
-        <v>zZY</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="8"/>
-        <v>ZY</v>
-      </c>
-      <c r="K16" t="str">
-        <f t="shared" si="9"/>
-        <v>XYZZY</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="11"/>
@@ -1449,47 +1758,48 @@
         <v>1</v>
       </c>
       <c r="B17" t="str">
+        <f t="shared" si="1"/>
+        <v>TRUE</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="2"/>
+        <v>TRUE</v>
+      </c>
+      <c r="D17" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="4"/>
+        <v>TR</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="6"/>
+        <v>true</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="7"/>
+        <v>T</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="8"/>
+        <v>zE</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="9"/>
+        <v>UE</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="10"/>
+        <v>TRUE</v>
+      </c>
+      <c r="L17" t="str">
         <f t="shared" si="0"/>
         <v>TRUE</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="1"/>
-        <v>TRUE</v>
-      </c>
-      <c r="D17" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E17" t="str">
-        <f t="shared" si="3"/>
-        <v>TR</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="G17" t="str">
-        <f t="shared" si="5"/>
-        <v>true</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" si="6"/>
-        <v>T</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="7"/>
-        <v>zE</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="8"/>
-        <v>UE</v>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="9"/>
-        <v>TRUE</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="11"/>
@@ -1509,47 +1819,48 @@
         <v>0</v>
       </c>
       <c r="B18" t="str">
+        <f t="shared" si="1"/>
+        <v>FALSE</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="2"/>
+        <v>FALSE</v>
+      </c>
+      <c r="D18" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="4"/>
+        <v>FA</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="6"/>
+        <v>false</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="7"/>
+        <v>F</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="8"/>
+        <v>zSE</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="9"/>
+        <v>SE</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="10"/>
+        <v>FALSE</v>
+      </c>
+      <c r="L18" t="str">
         <f t="shared" si="0"/>
         <v>FALSE</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="D18" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E18" t="str">
-        <f t="shared" si="3"/>
-        <v>FA</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="5"/>
-        <v>false</v>
-      </c>
-      <c r="H18" t="str">
-        <f t="shared" si="6"/>
-        <v>F</v>
-      </c>
-      <c r="I18" t="str">
-        <f t="shared" si="7"/>
-        <v>zSE</v>
-      </c>
-      <c r="J18" t="str">
-        <f t="shared" si="8"/>
-        <v>SE</v>
-      </c>
-      <c r="K18" t="str">
-        <f t="shared" si="9"/>
-        <v>FALSE</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="11"/>
@@ -1569,47 +1880,48 @@
         <v>1.23</v>
       </c>
       <c r="B19" t="str">
+        <f t="shared" si="1"/>
+        <v>1.23</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="2"/>
+        <v>1.23</v>
+      </c>
+      <c r="D19" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="4"/>
+        <v>1.</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="6"/>
+        <v>1.23</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="8"/>
+        <v>z3</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="9"/>
+        <v>23</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="10"/>
+        <v>1.23</v>
+      </c>
+      <c r="L19" t="str">
         <f t="shared" si="0"/>
         <v>1.23</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="1"/>
-        <v>1.23</v>
-      </c>
-      <c r="D19" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" t="str">
-        <f t="shared" si="3"/>
-        <v>1.</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" si="5"/>
-        <v>1.23</v>
-      </c>
-      <c r="H19" t="str">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="7"/>
-        <v>z3</v>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="8"/>
-        <v>23</v>
-      </c>
-      <c r="K19" t="str">
-        <f t="shared" si="9"/>
-        <v>1.23</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="11"/>
@@ -1629,47 +1941,48 @@
         <v>-2.34</v>
       </c>
       <c r="B20" t="str">
+        <f t="shared" si="1"/>
+        <v>-2.34</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="2"/>
+        <v>-2.34</v>
+      </c>
+      <c r="D20" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="6"/>
+        <v>-2.34</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="8"/>
+        <v>z34</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="9"/>
+        <v>34</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="10"/>
+        <v>-2.34</v>
+      </c>
+      <c r="L20" t="str">
         <f t="shared" si="0"/>
         <v>-2.34</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="1"/>
-        <v>-2.34</v>
-      </c>
-      <c r="D20" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E20" t="str">
-        <f t="shared" si="3"/>
-        <v>-2</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="G20" t="str">
-        <f t="shared" si="5"/>
-        <v>-2.34</v>
-      </c>
-      <c r="H20" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="7"/>
-        <v>z34</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="8"/>
-        <v>34</v>
-      </c>
-      <c r="K20" t="str">
-        <f t="shared" si="9"/>
-        <v>-2.34</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="11"/>
@@ -1689,47 +2002,48 @@
         <v>36526</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>36526</v>
-      </c>
-      <c r="C21" t="str">
         <f t="shared" si="1"/>
         <v>36526</v>
       </c>
+      <c r="C21" t="str">
+        <f t="shared" si="2"/>
+        <v>36526</v>
+      </c>
       <c r="D21" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="F21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>36526</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>z26</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>26</v>
       </c>
       <c r="K21" t="str">
         <f>SUBSTITUTE(A21,"6", "q",2)</f>
         <v>3652q</v>
       </c>
-      <c r="L21" s="4" t="s">
-        <v>17</v>
+      <c r="L21" t="str">
+        <f t="shared" si="0"/>
+        <v>36526.</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="11"/>
@@ -1746,6 +2060,1438 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02EDF0B-2538-4E3D-87EA-BE651753CF7C}">
+  <dimension ref="A1:D49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="str">
+        <f>TEXT(A2,B2)</f>
+        <v>938803</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="str">
+        <f>TEXT(A3,B3)</f>
+        <v>56328188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="str">
+        <f>TEXT(A4,B4)</f>
+        <v>3379691287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="str">
+        <f>TEXT(A5,B5)</f>
+        <v>-  1.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="str">
+        <f>TEXT(A6,B6)</f>
+        <v>ZERO</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="str">
+        <f>TEXT(A7,B7)</f>
+        <v>1.00</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="str">
+        <f>TEXT(A8,B8)</f>
+        <v>-&gt;X&lt;-X</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="e">
+        <f>TEXT(A9,B9)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="str">
+        <f>TEXT(A10,B10)</f>
+        <v>SS1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2958465</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="str">
+        <f>TEXT(A11,B11)</f>
+        <v>71003160</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>71003160</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="str">
+        <f>TEXT(A12,B12)</f>
+        <v>1704075840</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>71003160/24+1</f>
+        <v>2958466</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="str">
+        <f>TEXT(A13,B13)</f>
+        <v>71003184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>71003160/24+1</f>
+        <v>2958466</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="e">
+        <f>TEXT(A14,B14)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>71003160/24+1</f>
+        <v>2958466</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="e">
+        <f>TEXT(A15,B15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>71003160/24</f>
+        <v>2958465</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="str">
+        <f>TEXT(A16,B16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>71003160/24+1</f>
+        <v>2958466</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="e">
+        <f>TEXT(A17,B17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="str">
+        <f>TEXT(A18,B18)</f>
+        <v>-24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="e">
+        <f>TEXT(A19,B19)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="str">
+        <f>TEXT(A20,B20)</f>
+        <v>0:0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="e">
+        <f>TEXT(A21,B21)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="str">
+        <f>TEXT(A22,B22)</f>
+        <v>-1440</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>-1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="e">
+        <f>TEXT(A23,B23)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="str">
+        <f>TEXT(A24,B24)</f>
+        <v>0:0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>-1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="e">
+        <f>TEXT(A25,B25)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>-1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="str">
+        <f>TEXT(A26,B26)</f>
+        <v>-86400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>-1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="e">
+        <f>TEXT(A27,B27)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="str">
+        <f>TEXT(A28,B28)</f>
+        <v>0.000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>-1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="e">
+        <f>TEXT(A29,B29)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="str">
+        <f>TEXT(A30,B30)</f>
+        <v>.04212</v>
+      </c>
+      <c r="D30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="str">
+        <f>TEXT(A31,B31)</f>
+        <v>60:99</v>
+      </c>
+      <c r="D31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="str">
+        <f>TEXT(A32,B32)</f>
+        <v>1.02708</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="str">
+        <f>TEXT(A33,B33)</f>
+        <v>24:99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="str">
+        <f>TEXT(A34,B34)</f>
+        <v>7.90208</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" t="str">
+        <f>TEXT(A35,B35)</f>
+        <v>23:10000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="str">
+        <f>TEXT(A36,B36)</f>
+        <v>.11573</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" t="str">
+        <f>TEXT(A37,B37)</f>
+        <v>0:0:10000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" t="str">
+        <f>TEXT(A38,B38)</f>
+        <v>1.11503</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" t="str">
+        <f>TEXT(A39,B39)</f>
+        <v>23:60:9999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" t="str">
+        <f>TEXT(A40,B40)</f>
+        <v>.1567</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" t="str">
+        <f>TEXT(A41,B41)</f>
+        <v>59:10000.0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" t="str">
+        <f>TEXT(A42,B42)</f>
+        <v>.0166552</v>
+      </c>
+      <c r="D42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" t="str">
+        <f>TEXT(A43,B43)</f>
+        <v>0.15670153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" t="str">
+        <f>TEXT(A44,B44)</f>
+        <v>60:9999.012345</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" t="str">
+        <f>TEXT(A45,B45)</f>
+        <v>.15670153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="str">
+        <f>TEXT(A46,B46)</f>
+        <v>23:59.:0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="str">
+        <f>TEXT(A47,B47)</f>
+        <v>.99930555556</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" t="str">
+        <f>TEXT(A48,B48)</f>
+        <v>23.:59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>-1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" t="e">
+        <f>TEXT(A49,B49)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" display="&quot;hh&quot;@" xr:uid="{16DDCCA3-1D55-4380-8BE9-413D77EF1633}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E78BE6-503A-4FD4-A79D-BEE82BDE82D2}">
+  <dimension ref="A1:D68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1234567.8899999999</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="str">
+        <f>TEXT(A2,B2)</f>
+        <v>1,234,56ZZ7.8YY90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="e">
+        <f>TEXT(A3,B3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="e">
+        <f>TEXT(A4,B4)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="e">
+        <f>TEXT(A5,B5)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="str">
+        <f>TEXT(A6,B6)</f>
+        <v>ZZ.0z00</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="str">
+        <f>TEXT(A7,B7)</f>
+        <v>x</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="str">
+        <f>TEXT(A8,B8)</f>
+        <v>w</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="str">
+        <f>TEXT(A9,B9)</f>
+        <v>w</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="str">
+        <f>TEXT(A10,B10)</f>
+        <v>x</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="str">
+        <f>TEXT(A11,B11)</f>
+        <v>z</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="str">
+        <f>TEXT(A12,B12)</f>
+        <v>w</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-1</v>
+      </c>
+      <c r="C13" t="str">
+        <f>TEXT(A13,B13)</f>
+        <v>-</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="str">
+        <f>TEXT(A14,B14)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="str">
+        <f>TEXT(A15,B15)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="str">
+        <f>TEXT(A16,B16)</f>
+        <v>Plugh</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="str">
+        <f>TEXT(A17,B17)</f>
+        <v>-w</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="str">
+        <f>TEXT(A18,B18)</f>
+        <v>w</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="str">
+        <f>TEXT(A19,B19)</f>
+        <v>w</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="str">
+        <f>TEXT(A21,B21)</f>
+        <v>890123.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" t="str">
+        <f>TEXT(A22,B22)</f>
+        <v>890123.46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" t="str">
+        <f>TEXT(A23,B23)</f>
+        <v>890123.457</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="str">
+        <f>TEXT(A24,B24)</f>
+        <v>890123.457.</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="str">
+        <f>TEXT(A25,B25)</f>
+        <v>890123.456.7.8.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" ref="C26:C34" si="0">TEXT(A26,B26)</f>
+        <v>890123.456.78.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>890,123.45.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>890,123.45.68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>890,123.45.679</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>890,123.45.679</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>890,123.45.67,9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>890,123.45.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>890,123.45.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>89012x3.45.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" ref="C35:C44" si="1">TEXT(A35,B35)</f>
+        <v>890,12x3.45.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="1"/>
+        <v>8901x,2x3.45.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B37" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="1"/>
+        <v>890,1x,23.45.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="1"/>
+        <v>,890123.45.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="1"/>
+        <v>890123.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="1"/>
+        <v>890123.456x,79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="1"/>
+        <v>890123.456x79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="1"/>
+        <v>890123.456x,79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="1"/>
+        <v>890123.456x,79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="1"/>
+        <v>89012346%</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" ref="C45:C49" si="2">TEXT(A45,B45)</f>
+        <v>89012345.7%</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="2"/>
+        <v>8901234%6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="2"/>
+        <v>%89012346</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B48" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="2"/>
+        <v>%89012345678%9%</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B49" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="2"/>
+        <v>%890123456789%0%0%</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="B50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" ref="C50:C56" si="3">TEXT(A50,B50)</f>
+        <v>890123.45678900</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>890123.45678899996</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" ref="C57:C64" si="4">TEXT(A57,B57)</f>
+        <v>1.</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="4"/>
+        <v>1.</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="4"/>
+        <v>1.</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="4"/>
+        <v>1.</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B61" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="4"/>
+        <v>1.</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D62">
+        <f>LEN(C62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1234.56</v>
+      </c>
+      <c r="B63" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="4"/>
+        <v>$x1,235</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1234.56</v>
+      </c>
+      <c r="B64" t="s">
+        <v>97</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" ref="C64" si="5">TEXT(A64,B64)</f>
+        <v>1234.6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1234.56</v>
+      </c>
+      <c r="B65" t="s">
+        <v>117</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" ref="C65:C68" si="6">TEXT(A65,B65)</f>
+        <v>1234.56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1234.56</v>
+      </c>
+      <c r="B66" t="s">
+        <v>118</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="6"/>
+        <v>1234.560</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>-1</v>
+      </c>
+      <c r="B67" t="s">
+        <v>114</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="6"/>
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>